<commit_message>
Updated with version numbers, updated JSON structure, refined codests
</commit_message>
<xml_diff>
--- a/xlsx/access-type.xlsx
+++ b/xlsx/access-type.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -21,6 +24,9 @@
   </si>
   <si>
     <t xml:space="preserve">Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0</t>
   </si>
   <si>
     <t xml:space="preserve">O</t>
@@ -377,7 +383,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -389,38 +395,50 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>